<commit_message>
Integrate Agora data for elec/TCAMRB, elec/TCCpUCD, and elec/WUbPPT
</commit_message>
<xml_diff>
--- a/InputData/elec/WUbPPT/Water Use by Power Plant Type.xlsx
+++ b/InputData/elec/WUbPPT/Water Use by Power Plant Type.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\WUbPPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\2020\2020-04_EPS_Europe\30_Forschung_(intern)\InputData_EU28\elec\WUbPPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE6A0DD-CD15-4D83-8231-72F12AD7FDCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="34776" windowHeight="19056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="WUbPPT-withdrawals" sheetId="6" r:id="rId6"/>
     <sheet name="WUbPPT-consumption" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -299,7 +300,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,8 +377,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -654,22 +655,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -677,127 +678,130 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>10^12</f>
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>277777777.77777702</v>
       </c>
     </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -805,13 +809,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.3984375" customWidth="1"/>
-    <col min="4" max="4" width="27.3984375" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -891,7 +895,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -971,7 +975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1055,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1131,7 +1135,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1215,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1455,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1691,7 +1695,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +1775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1935,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2091,7 +2095,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2255,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2331,7 +2335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2571,7 +2575,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2731,7 +2735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2817,7 +2821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2825,15 +2829,15 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" customWidth="1"/>
-    <col min="5" max="5" width="29.265625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -2919,7 +2923,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3091,7 +3095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3177,7 +3181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -3263,7 +3267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -3349,7 +3353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3435,7 +3439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -3521,7 +3525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -3607,7 +3611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -3693,7 +3697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -3779,7 +3783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -3865,7 +3869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -3951,7 +3955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4037,7 +4041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4123,7 +4127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -4215,23 +4219,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="4" max="4" width="17.1328125" customWidth="1"/>
-    <col min="5" max="5" width="27.73046875" customWidth="1"/>
-    <col min="6" max="6" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -4317,7 +4321,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4403,7 +4407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4489,7 +4493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4575,7 +4579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4661,7 +4665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -4747,7 +4751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4833,7 +4837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4919,7 +4923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -5005,7 +5009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -5091,7 +5095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -5177,7 +5181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -5263,7 +5267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -5349,7 +5353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -5435,7 +5439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -5521,7 +5525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -5607,7 +5611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -5700,24 +5704,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" customWidth="1"/>
-    <col min="3" max="3" width="27.265625" customWidth="1"/>
-    <col min="4" max="4" width="27.3984375" customWidth="1"/>
-    <col min="5" max="5" width="29.265625" customWidth="1"/>
-    <col min="6" max="8" width="28.59765625" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29.21875" customWidth="1"/>
+    <col min="6" max="8" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -5743,7 +5747,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -5776,7 +5780,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5809,7 +5813,7 @@
         <v>971.73432153190504</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5842,7 +5846,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5875,7 +5879,7 @@
         <v>1960.1218806510001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -5908,7 +5912,7 @@
         <v>620.64013917559782</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -5941,7 +5945,7 @@
         <v>745.03641899418494</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5974,7 +5978,7 @@
         <v>4930.3337614825323</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -6003,7 +6007,7 @@
         <v>16999.982182329317</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6036,7 +6040,7 @@
         <v>2226.6884419345611</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -6069,7 +6073,7 @@
         <v>1684.774202794702</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -6102,7 +6106,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -6135,7 +6139,7 @@
         <v>1183.8566612430841</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -6168,7 +6172,7 @@
         <v>2103.5281074696754</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -6201,7 +6205,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -6234,7 +6238,7 @@
         <v>20.000187272534593</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -6273,28 +6277,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" customWidth="1"/>
+    <col min="1" max="1" width="24.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -6303,7 +6307,7 @@
         <v>54577.83755331373</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -6312,7 +6316,7 @@
         <v>4159.9245358989992</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -6321,7 +6325,7 @@
         <v>63249.562164099065</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -6330,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -6338,7 +6342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -6347,7 +6351,7 @@
         <v>20.000187272534593</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -6356,7 +6360,7 @@
         <v>2103.5281074696754</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -6365,7 +6369,7 @@
         <v>13890.685457654999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -6374,7 +6378,7 @@
         <v>4930.3337614825323</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -6383,7 +6387,7 @@
         <v>23313.172724314474</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -6392,7 +6396,7 @@
         <v>30331.387156235895</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -6401,7 +6405,7 @@
         <v>54577.83755331373</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -6409,7 +6413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -6418,7 +6422,7 @@
         <v>23313.172724314474</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -6427,7 +6431,7 @@
         <v>23313.172724314474</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -6442,28 +6446,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" customWidth="1"/>
+    <col min="1" max="1" width="24.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -6472,7 +6474,7 @@
         <v>1960.1218806510001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -6481,7 +6483,7 @@
         <v>620.64013917559782</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -6490,7 +6492,7 @@
         <v>1684.774202794702</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -6499,7 +6501,7 @@
         <v>16999.982182329317</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -6507,16 +6509,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="6">
-        <f>'2015 Consolidated Data'!H16</f>
-        <v>20.000187272534593</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -6525,7 +6526,7 @@
         <v>2103.5281074696754</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -6534,7 +6535,7 @@
         <v>971.73432153190504</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -6543,7 +6544,7 @@
         <v>4930.3337614825323</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -6552,7 +6553,7 @@
         <v>1183.8566612430841</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -6561,7 +6562,7 @@
         <v>745.03641899418494</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -6570,7 +6571,7 @@
         <v>1960.1218806510001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -6578,7 +6579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -6587,7 +6588,7 @@
         <v>1183.8566612430841</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -6596,7 +6597,7 @@
         <v>1183.8566612430841</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>85</v>
       </c>

</xml_diff>